<commit_message>
aggiunti metodi con calcolo del delta
</commit_message>
<xml_diff>
--- a/OptimizationTimes.xlsx
+++ b/OptimizationTimes.xlsx
@@ -1,41 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finix\Dropbox\Lavoro\Universita\Dottorato\Courses\Efficient implementation of local search and metaheuristics in Cpp\Final Project\Euristics-and-Methaeuristics---Bruno---2024\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB249FB-BC93-495A-B57F-4463136734B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Marco" sheetId="1" r:id="rId1"/>
+    <sheet name="Salvo" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Salvo!$A$1:$G$3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>d493</t>
+  </si>
+  <si>
+    <t>64251ms</t>
+  </si>
+  <si>
+    <t>Original Method</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ali535</t>
+  </si>
+  <si>
+    <t>Initial value</t>
+  </si>
+  <si>
+    <t>With delta evaluetion</t>
+  </si>
+  <si>
+    <t>Time ms</t>
+  </si>
+  <si>
+    <t>Initial time ms</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,17 +112,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,37 +461,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.69921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Instance</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Time</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Method</v>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>d493</v>
-      </c>
-      <c r="B2" t="str">
-        <v>64251ms</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Original Method</v>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError sqref="A1:C2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844F34F5-D4EB-442B-B09E-BAB911F7391F}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="6" width="11.3984375" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>253127</v>
+      </c>
+      <c r="D2" s="2">
+        <v>58548</v>
+      </c>
+      <c r="E2" s="2">
+        <v>230423</v>
+      </c>
+      <c r="F2" s="1">
+        <f>(E2-C2)/(D2-B2)</f>
+        <v>-0.3878440014349408</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>41665</v>
+      </c>
+      <c r="D3" s="2">
+        <v>39836</v>
+      </c>
+      <c r="E3" s="2">
+        <v>38548</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(E3-C3)/(D3-B3)</f>
+        <v>-7.8259559617364235E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G3" xr:uid="{844F34F5-D4EB-442B-B09E-BAB911F7391F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tabella tempi e valori aggiornata
</commit_message>
<xml_diff>
--- a/OptimizationTimes.xlsx
+++ b/OptimizationTimes.xlsx
@@ -5,24 +5,40 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Euristics-and-Methaeuristics---Bruno---2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finix\Dropbox\Lavoro\Universita\Dottorato\Courses\Efficient implementation of local search and metaheuristics in Cpp\Final Project\Euristics-and-Methaeuristics---Bruno---2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F44E4C-8640-414B-B208-2013C4D91CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19638D25-7DFF-4FCB-864D-D19600E5EE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marco" sheetId="1" r:id="rId1"/>
     <sheet name="Salvo" sheetId="2" r:id="rId2"/>
     <sheet name="General Computational Results" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Salvo!$A$1:$G$15</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Instance</t>
   </si>
@@ -57,39 +73,6 @@
     <t>ali535</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>253127</t>
-  </si>
-  <si>
-    <t>58548</t>
-  </si>
-  <si>
-    <t>230423</t>
-  </si>
-  <si>
-    <t>-39%</t>
-  </si>
-  <si>
-    <t>With delta evaluetion</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>41665</t>
-  </si>
-  <si>
-    <t>39836</t>
-  </si>
-  <si>
-    <t>38548</t>
-  </si>
-  <si>
-    <t>-8%</t>
-  </si>
-  <si>
     <t>GreSol</t>
   </si>
   <si>
@@ -109,13 +92,25 @@
   </si>
   <si>
     <t>att48</t>
+  </si>
+  <si>
+    <t>Gain?</t>
+  </si>
+  <si>
+    <t>With delta evaluation Salvo</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>With delta evaluation Marco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,6 +120,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -164,16 +166,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -514,9 +522,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -548,15 +556,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="6" width="11.3984375" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,61 +587,352 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="3">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3">
+        <v>253127</v>
+      </c>
+      <c r="D2" s="3">
+        <v>30345</v>
+      </c>
+      <c r="E2" s="3">
+        <v>225158</v>
+      </c>
+      <c r="F2" s="4">
+        <f t="shared" ref="F2:F15" si="0">(C2-E2)/(D2-B2)</f>
+        <v>0.92197389240506333</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>253127</v>
+      </c>
+      <c r="D3" s="3">
+        <v>171183</v>
+      </c>
+      <c r="E3" s="3">
+        <v>218438</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2026546242690144</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>253127</v>
+      </c>
+      <c r="D4" s="3">
+        <v>135447</v>
+      </c>
+      <c r="E4" s="3">
+        <v>222359</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22717405750232578</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>12861</v>
+      </c>
+      <c r="D5" s="3">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10906</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>12861</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>11643</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>406</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>12861</v>
+      </c>
+      <c r="D7" s="3">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E7" s="3">
+        <v>11100</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>125.78571428571429</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5919</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5715</v>
+      </c>
+      <c r="F8" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5919</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5879</v>
+      </c>
+      <c r="F9" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5919</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5715</v>
+      </c>
+      <c r="F10" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2005</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1643</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2005</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1815</v>
+      </c>
+      <c r="F12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2005</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1722</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>41665</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1925</v>
+      </c>
+      <c r="E14" s="3">
+        <v>38059</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8800834202294057</v>
+      </c>
+      <c r="G14" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>41665</v>
+      </c>
+      <c r="D15" s="3">
+        <v>111394</v>
+      </c>
+      <c r="E15" s="3">
+        <v>36569</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5749991022372247E-2</v>
+      </c>
+      <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G15" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:G3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -638,56 +944,56 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="14.125" customWidth="1"/>
+    <col min="1" max="5" width="14.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -696,7 +1002,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>